<commit_message>
change max vol in normalisation.py
</commit_message>
<xml_diff>
--- a/pciogreen_pcr-20200414-xr.xlsx
+++ b/pciogreen_pcr-20200414-xr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattstorey/opentrons_protocols/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EE5DDB-1B8C-CC4E-91B2-C66E653E642D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565B1835-5571-C043-A16D-EC0EFB5C1463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1675,7 +1675,7 @@
   <dimension ref="A3:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:D23"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1773,12 +1773,8 @@
       <c r="B16" s="3">
         <v>40000</v>
       </c>
-      <c r="C16" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D16" s="3">
-        <v>40000</v>
-      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="4">
         <v>121</v>
       </c>
@@ -1796,14 +1792,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="3">
-        <v>40000</v>
-      </c>
-      <c r="C17" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D17" s="3">
-        <v>40000</v>
-      </c>
+        <v>20000</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="6">
         <v>43244</v>
       </c>
@@ -1821,14 +1813,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="3">
-        <v>40000</v>
-      </c>
-      <c r="C18" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D18" s="3">
-        <v>40000</v>
-      </c>
+        <v>10000</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="6">
         <v>5330</v>
       </c>
@@ -1846,14 +1834,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="3">
-        <v>40000</v>
-      </c>
-      <c r="C19" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D19" s="3">
-        <v>40000</v>
-      </c>
+        <v>5000</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
       <c r="E19" s="6">
         <v>709</v>
       </c>
@@ -1871,14 +1855,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="3">
-        <v>40000</v>
-      </c>
-      <c r="C20" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D20" s="3">
-        <v>40000</v>
-      </c>
+        <v>4000</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="6">
         <v>186</v>
       </c>
@@ -1896,14 +1876,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="3">
-        <v>40000</v>
-      </c>
-      <c r="C21" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D21" s="3">
-        <v>40000</v>
-      </c>
+        <v>3000</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -1919,14 +1895,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="3">
-        <v>40000</v>
-      </c>
-      <c r="C22" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D22" s="3">
-        <v>40000</v>
-      </c>
+        <v>2000</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -1942,14 +1914,10 @@
         <v>16</v>
       </c>
       <c r="B23" s="3">
-        <v>40000</v>
-      </c>
-      <c r="C23" s="3">
-        <v>40000</v>
-      </c>
-      <c r="D23" s="3">
-        <v>40000</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>

</xml_diff>